<commit_message>
separate out app and outstation; add loader, options and mqtt_wrapper
</commit_message>
<xml_diff>
--- a/CCT_protocol_spec.xlsx
+++ b/CCT_protocol_spec.xlsx
@@ -1067,7 +1067,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1180,22 +1180,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1226,10 +1210,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -1511,11 +1491,11 @@
   </sheetPr>
   <dimension ref="B1:M88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.28"/>
@@ -1973,34 +1953,34 @@
       <c r="B18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="29" t="n">
+      <c r="E18" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="29" t="n">
+      <c r="G18" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="29" t="n">
+      <c r="H18" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="31" t="n">
+      <c r="I18" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="J18" s="29" t="n">
+      <c r="J18" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="K18" s="29" t="n">
+      <c r="K18" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="L18" s="31" t="n">
+      <c r="L18" s="19" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2008,115 +1988,115 @@
       <c r="B19" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="29" t="n">
+      <c r="E19" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="29" t="n">
+      <c r="G19" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="H19" s="29" t="n">
+      <c r="H19" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="31" t="n">
+      <c r="I19" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="J19" s="29" t="n">
+      <c r="J19" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="K19" s="29" t="n">
+      <c r="K19" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="L19" s="31" t="n">
+      <c r="L19" s="19" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34" t="s">
+      <c r="E20" s="29"/>
+      <c r="F20" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="36" t="s">
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="L20" s="36"/>
+      <c r="L20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="38"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="38"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="34"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="4" t="s">
         <v>54</v>
       </c>
@@ -2128,208 +2108,208 @@
       <c r="L24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="50"/>
-      <c r="F25" s="47" t="s">
+      <c r="E25" s="45"/>
+      <c r="F25" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="51" t="s">
+      <c r="G25" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="49" t="s">
+      <c r="H25" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="52" t="n">
+      <c r="B26" s="47" t="n">
         <v>30</v>
       </c>
-      <c r="C26" s="53" t="n">
+      <c r="C26" s="48" t="n">
         <v>4</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="55"/>
-      <c r="F26" s="52" t="n">
+      <c r="E26" s="50"/>
+      <c r="F26" s="47" t="n">
         <v>41</v>
       </c>
-      <c r="G26" s="56" t="n">
+      <c r="G26" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="H26" s="57" t="s">
+      <c r="H26" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="52"/>
-      <c r="C27" s="53" t="n">
+      <c r="B27" s="47"/>
+      <c r="C27" s="48" t="n">
         <v>5</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="55"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="63"/>
-      <c r="L28" s="63"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="52" t="n">
+      <c r="B29" s="47" t="n">
         <v>32</v>
       </c>
-      <c r="C29" s="53" t="n">
+      <c r="C29" s="48" t="n">
         <v>4</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="D29" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="55"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="64"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="59"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="52"/>
-      <c r="C30" s="53" t="n">
+      <c r="B30" s="47"/>
+      <c r="C30" s="48" t="n">
         <v>7</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D30" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="E30" s="55"/>
-      <c r="F30" s="65" t="s">
+      <c r="E30" s="50"/>
+      <c r="F30" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="65" t="s">
+      <c r="E31" s="55"/>
+      <c r="F31" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="66" t="n">
+      <c r="B32" s="61" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="53" t="n">
+      <c r="C32" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="67" t="s">
+      <c r="E32" s="50"/>
+      <c r="F32" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="68"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="63"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="64"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="59"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="66" t="n">
+      <c r="B34" s="61" t="n">
         <v>2</v>
       </c>
-      <c r="C34" s="53" t="n">
+      <c r="C34" s="48" t="n">
         <v>2</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="D34" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="55"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="64"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="59"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="71"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="65"/>
+      <c r="L35" s="66"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
     </row>
     <row r="37" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2375,14 +2355,14 @@
       <c r="I55" s="18"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-      <c r="I56" s="29"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-      <c r="I57" s="29"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2477,7 +2457,7 @@
       <selection pane="topLeft" activeCell="M35" activeCellId="0" sqref="M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.86"/>
@@ -2486,889 +2466,889 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="76"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="78"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="73"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="79"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="80"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
+      <c r="C13" s="76"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="74" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="77"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="79"/>
+      <c r="I19" s="79"/>
+      <c r="J19" s="79"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="77"/>
+      <c r="L20" s="77"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="79"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="85" t="s">
+      <c r="B22" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="85"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="85"/>
-      <c r="K22" s="85"/>
-      <c r="L22" s="85"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+      <c r="L22" s="80"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="79"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="86"/>
-      <c r="K24" s="86"/>
-      <c r="L24" s="86"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="74"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="79" t="s">
+      <c r="B26" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="79"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="79" t="s">
+      <c r="B28" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="79"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+      <c r="K28" s="74"/>
+      <c r="L28" s="74"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="79"/>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
-      <c r="H30" s="79"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
-      <c r="K30" s="79"/>
-      <c r="L30" s="79"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="79" t="s">
+      <c r="B31" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="74"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="79" t="s">
+      <c r="B32" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="79"/>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="79"/>
-      <c r="J32" s="79"/>
-      <c r="K32" s="79"/>
-      <c r="L32" s="79"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="74"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="74" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="79"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="79" t="s">
+      <c r="B34" s="74" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="79" t="s">
+      <c r="B36" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="79"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="79"/>
-      <c r="F37" s="79"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="79" t="s">
+      <c r="B38" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="79"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="74"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="74"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="87" t="s">
+      <c r="B40" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="C40" s="87"/>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="87"/>
-      <c r="J40" s="87"/>
-      <c r="K40" s="87"/>
-      <c r="L40" s="87"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="82"/>
+      <c r="J40" s="82"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="79" t="s">
+      <c r="B41" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="79"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="74"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="79"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="79"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="79"/>
-      <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="79"/>
-      <c r="J42" s="79"/>
-      <c r="K42" s="79"/>
-      <c r="L42" s="79"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="79" t="s">
+      <c r="B43" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="74"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="79" t="s">
+      <c r="B44" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="79"/>
-      <c r="D44" s="79"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="79"/>
-      <c r="G44" s="79"/>
-      <c r="H44" s="79"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="79"/>
-      <c r="L44" s="79"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="79"/>
-      <c r="G45" s="79"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="74"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="74"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="79"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="79"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="79"/>
-      <c r="G46" s="79"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="79"/>
-      <c r="J46" s="79"/>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="74"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="85" t="s">
+      <c r="B47" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
-      <c r="I47" s="85"/>
-      <c r="J47" s="85"/>
-      <c r="K47" s="85"/>
-      <c r="L47" s="85"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="80"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="80"/>
+      <c r="H47" s="80"/>
+      <c r="I47" s="80"/>
+      <c r="J47" s="80"/>
+      <c r="K47" s="80"/>
+      <c r="L47" s="80"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="79" t="s">
+      <c r="B48" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="79"/>
-      <c r="D48" s="79"/>
-      <c r="E48" s="79"/>
-      <c r="F48" s="79"/>
-      <c r="G48" s="79"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="79"/>
-      <c r="J48" s="79"/>
-      <c r="K48" s="79"/>
-      <c r="L48" s="79"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="74"/>
+      <c r="L48" s="74"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="79"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="79"/>
-      <c r="F49" s="79"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="74"/>
+      <c r="J49" s="74"/>
+      <c r="K49" s="74"/>
+      <c r="L49" s="74"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
-      <c r="I50" s="85"/>
-      <c r="J50" s="85"/>
-      <c r="K50" s="85"/>
-      <c r="L50" s="85"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="80"/>
+      <c r="H50" s="80"/>
+      <c r="I50" s="80"/>
+      <c r="J50" s="80"/>
+      <c r="K50" s="80"/>
+      <c r="L50" s="80"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="79" t="s">
+      <c r="B51" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="79"/>
-      <c r="D51" s="79"/>
-      <c r="E51" s="79"/>
-      <c r="F51" s="79"/>
-      <c r="G51" s="79"/>
-      <c r="H51" s="79"/>
-      <c r="I51" s="79"/>
-      <c r="J51" s="79"/>
-      <c r="K51" s="79"/>
-      <c r="L51" s="79"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="74"/>
+      <c r="J51" s="74"/>
+      <c r="K51" s="74"/>
+      <c r="L51" s="74"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="79" t="s">
+      <c r="B52" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="79"/>
-      <c r="D52" s="79"/>
-      <c r="E52" s="79"/>
-      <c r="F52" s="79"/>
-      <c r="G52" s="79"/>
-      <c r="H52" s="79"/>
-      <c r="I52" s="79"/>
-      <c r="J52" s="79"/>
-      <c r="K52" s="79"/>
-      <c r="L52" s="79"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
+      <c r="I52" s="74"/>
+      <c r="J52" s="74"/>
+      <c r="K52" s="74"/>
+      <c r="L52" s="74"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="79"/>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="79"/>
+      <c r="B53" s="74"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
+      <c r="H53" s="74"/>
+      <c r="I53" s="74"/>
+      <c r="J53" s="74"/>
+      <c r="K53" s="74"/>
+      <c r="L53" s="74"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="85" t="s">
+      <c r="B54" s="80" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="85"/>
-      <c r="D54" s="85"/>
-      <c r="E54" s="85"/>
-      <c r="F54" s="85"/>
-      <c r="G54" s="85"/>
-      <c r="H54" s="85"/>
-      <c r="I54" s="85"/>
-      <c r="J54" s="85"/>
-      <c r="K54" s="85"/>
-      <c r="L54" s="85"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="80"/>
+      <c r="G54" s="80"/>
+      <c r="H54" s="80"/>
+      <c r="I54" s="80"/>
+      <c r="J54" s="80"/>
+      <c r="K54" s="80"/>
+      <c r="L54" s="80"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="79" t="s">
+      <c r="B55" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="79"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="79"/>
-      <c r="F55" s="79"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="74"/>
+      <c r="H55" s="74"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="74"/>
+      <c r="K55" s="74"/>
+      <c r="L55" s="74"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="79" t="s">
+      <c r="B56" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="79"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="79"/>
-      <c r="G56" s="79"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="79"/>
-      <c r="J56" s="79"/>
-      <c r="K56" s="79"/>
-      <c r="L56" s="79"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
+      <c r="F56" s="74"/>
+      <c r="G56" s="74"/>
+      <c r="H56" s="74"/>
+      <c r="I56" s="74"/>
+      <c r="J56" s="74"/>
+      <c r="K56" s="74"/>
+      <c r="L56" s="74"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="79"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="79"/>
-      <c r="E57" s="79"/>
-      <c r="F57" s="79"/>
-      <c r="G57" s="79"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="79"/>
-      <c r="J57" s="79"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="74"/>
+      <c r="G57" s="74"/>
+      <c r="H57" s="74"/>
+      <c r="I57" s="74"/>
+      <c r="J57" s="74"/>
+      <c r="K57" s="74"/>
+      <c r="L57" s="74"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="85" t="s">
+      <c r="B58" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="C58" s="85"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="85"/>
-      <c r="F58" s="85"/>
-      <c r="G58" s="85"/>
-      <c r="H58" s="85"/>
-      <c r="I58" s="85"/>
-      <c r="J58" s="85"/>
-      <c r="K58" s="85"/>
-      <c r="L58" s="85"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="80"/>
+      <c r="J58" s="80"/>
+      <c r="K58" s="80"/>
+      <c r="L58" s="80"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="79" t="s">
+      <c r="B59" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="79"/>
-      <c r="D59" s="79"/>
-      <c r="E59" s="79"/>
-      <c r="F59" s="79"/>
-      <c r="G59" s="79"/>
-      <c r="H59" s="79"/>
-      <c r="I59" s="79"/>
-      <c r="J59" s="79"/>
-      <c r="K59" s="79"/>
-      <c r="L59" s="79"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="74"/>
+      <c r="F59" s="74"/>
+      <c r="G59" s="74"/>
+      <c r="H59" s="74"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="74"/>
+      <c r="K59" s="74"/>
+      <c r="L59" s="74"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="88"/>
-      <c r="C60" s="88"/>
-      <c r="D60" s="88"/>
-      <c r="E60" s="88"/>
-      <c r="F60" s="88"/>
-      <c r="G60" s="88"/>
-      <c r="H60" s="88"/>
-      <c r="I60" s="88"/>
-      <c r="J60" s="88"/>
-      <c r="K60" s="88"/>
-      <c r="L60" s="88"/>
+      <c r="B60" s="83"/>
+      <c r="C60" s="83"/>
+      <c r="D60" s="83"/>
+      <c r="E60" s="83"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="83"/>
+      <c r="H60" s="83"/>
+      <c r="I60" s="83"/>
+      <c r="J60" s="83"/>
+      <c r="K60" s="83"/>
+      <c r="L60" s="83"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="89"/>
-      <c r="C61" s="89"/>
-      <c r="D61" s="89"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="89"/>
-      <c r="G61" s="89"/>
-      <c r="H61" s="89"/>
-      <c r="I61" s="90"/>
-      <c r="J61" s="90"/>
-      <c r="K61" s="90"/>
-      <c r="L61" s="38"/>
+      <c r="B61" s="84"/>
+      <c r="C61" s="84"/>
+      <c r="D61" s="84"/>
+      <c r="E61" s="84"/>
+      <c r="F61" s="84"/>
+      <c r="G61" s="84"/>
+      <c r="H61" s="84"/>
+      <c r="I61" s="85"/>
+      <c r="J61" s="85"/>
+      <c r="K61" s="85"/>
+      <c r="L61" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="59">

</xml_diff>

<commit_message>
add configurable buffer size
</commit_message>
<xml_diff>
--- a/CCT_protocol_spec.xlsx
+++ b/CCT_protocol_spec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="interopreability IO list" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="115">
   <si>
     <t xml:space="preserve">version  revision ref. SSEG Plant DNP3_SCADA_INTERFACE_2022_11_01.xlsx</t>
   </si>
@@ -509,19 +509,83 @@
     <t xml:space="preserve"> Test procedure to verify SSEG SCADA compliance .</t>
   </si>
   <si>
-    <t xml:space="preserve">1.  At the start of the tests the DNP3 Protocol validity attribute of all the configured inputs will be confirmed and must report as valid. (Any Input  that reports as Invalid will mean that the input was not correctly configured) </t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.  At the start of the tests the DNP3 Protocol </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">validity attribute</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> of all the configured inputs will be confirmed and must report as valid. (Any Input  that reports as Invalid will mean that the input was not correctly configured) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SOEHandler::Process()</t>
   </si>
   <si>
     <t xml:space="preserve">2.  Total Power Generated, Reactive Power and Exported/Imported Power  analogue values will be verified for accuracy and frequency that updates are received at the Client interface, in real time. These values performance will be monitored throughout the duration of the compliance tests.</t>
   </si>
   <si>
+    <t xml:space="preserve">VRAAG but polling is used?</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">3.  A  100% Production Constraint set point command will be sent from the DNP3 Client simulator  to the  DNP3 Server interface to increase  the energy production to  as much as the SSEG plant can produce at that time.  </t>
   </si>
   <si>
-    <t xml:space="preserve">   The  Total Power Generated analogue value  will be monitored as this value reported from the DNP3 Server Interface to the DNP3 Client simulator reaches its maximum value at which point the value stabilizes and</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">   The  Total Power Generated analogue value  will be monitored as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">this value </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reported from the DNP3 Server Interface to the DNP3 Client simulator reaches its maximum value at which point the value stabilizes and</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">   stops increasing. This value will determine what set points will be applied during the test procedure.</t>
@@ -678,7 +742,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -766,6 +830,13 @@
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC9211E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1475,7 +1546,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1491,15 +1562,15 @@
   </sheetPr>
   <dimension ref="B1:M88"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="87.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="83.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.28"/>
@@ -2451,13 +2522,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:L61"/>
+  <dimension ref="B1:M61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M35" activeCellId="0" sqref="M35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.39453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.86"/>
@@ -2465,7 +2536,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="166.85"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="68" t="s">
         <v>68</v>
       </c>
@@ -2510,7 +2581,7 @@
       <c r="K3" s="70"/>
       <c r="L3" s="70"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="70" t="s">
         <v>71</v>
       </c>
@@ -2555,7 +2626,7 @@
       <c r="K6" s="70"/>
       <c r="L6" s="70"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="71"/>
       <c r="C7" s="72"/>
       <c r="D7" s="72"/>
@@ -2568,7 +2639,7 @@
       <c r="K7" s="72"/>
       <c r="L7" s="73"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="70" t="s">
         <v>74</v>
       </c>
@@ -2583,7 +2654,7 @@
       <c r="K8" s="70"/>
       <c r="L8" s="70"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="70" t="s">
         <v>75</v>
       </c>
@@ -2613,7 +2684,7 @@
       <c r="K10" s="70"/>
       <c r="L10" s="70"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="74"/>
       <c r="C11" s="74"/>
       <c r="D11" s="74"/>
@@ -2626,7 +2697,7 @@
       <c r="K11" s="74"/>
       <c r="L11" s="74"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="75" t="s">
         <v>77</v>
       </c>
@@ -2641,7 +2712,7 @@
       <c r="K12" s="75"/>
       <c r="L12" s="75"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="76" t="s">
         <v>78</v>
       </c>
@@ -2656,7 +2727,7 @@
       <c r="K13" s="76"/>
       <c r="L13" s="76"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="74" t="s">
         <v>79</v>
       </c>
@@ -2671,7 +2742,7 @@
       <c r="K14" s="74"/>
       <c r="L14" s="74"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="76"/>
       <c r="C15" s="76"/>
       <c r="D15" s="76"/>
@@ -2684,7 +2755,7 @@
       <c r="K15" s="76"/>
       <c r="L15" s="76"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="76" t="s">
         <v>80</v>
       </c>
@@ -2699,7 +2770,7 @@
       <c r="K16" s="76"/>
       <c r="L16" s="76"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="77" t="s">
         <v>81</v>
       </c>
@@ -2714,7 +2785,7 @@
       <c r="K17" s="77"/>
       <c r="L17" s="77"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="78"/>
       <c r="C18" s="78"/>
       <c r="D18" s="78"/>
@@ -2727,7 +2798,7 @@
       <c r="K18" s="78"/>
       <c r="L18" s="78"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="79" t="s">
         <v>82</v>
       </c>
@@ -2742,7 +2813,7 @@
       <c r="K19" s="79"/>
       <c r="L19" s="79"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="77" t="s">
         <v>83</v>
       </c>
@@ -2757,7 +2828,7 @@
       <c r="K20" s="77"/>
       <c r="L20" s="77"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="74"/>
       <c r="C21" s="74"/>
       <c r="D21" s="74"/>
@@ -2770,7 +2841,7 @@
       <c r="K21" s="74"/>
       <c r="L21" s="74"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="80" t="s">
         <v>84</v>
       </c>
@@ -2785,7 +2856,7 @@
       <c r="K22" s="80"/>
       <c r="L22" s="80"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="74"/>
       <c r="C23" s="74"/>
       <c r="D23" s="74"/>
@@ -2798,7 +2869,7 @@
       <c r="K23" s="74"/>
       <c r="L23" s="74"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="81" t="s">
         <v>85</v>
       </c>
@@ -2813,7 +2884,7 @@
       <c r="K24" s="81"/>
       <c r="L24" s="81"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="74"/>
       <c r="C25" s="74"/>
       <c r="D25" s="74"/>
@@ -2826,7 +2897,7 @@
       <c r="K25" s="74"/>
       <c r="L25" s="74"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="74" t="s">
         <v>86</v>
       </c>
@@ -2840,8 +2911,11 @@
       <c r="J26" s="74"/>
       <c r="K26" s="74"/>
       <c r="L26" s="74"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="74"/>
       <c r="C27" s="74"/>
       <c r="D27" s="74"/>
@@ -2854,9 +2928,9 @@
       <c r="K27" s="74"/>
       <c r="L27" s="74"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="74" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C28" s="74"/>
       <c r="D28" s="74"/>
@@ -2868,10 +2942,13 @@
       <c r="J28" s="74"/>
       <c r="K28" s="74"/>
       <c r="L28" s="74"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M28" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="74" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C29" s="74"/>
       <c r="D29" s="74"/>
@@ -2884,9 +2961,9 @@
       <c r="K29" s="74"/>
       <c r="L29" s="74"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="74" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C30" s="74"/>
       <c r="D30" s="74"/>
@@ -2899,9 +2976,9 @@
       <c r="K30" s="74"/>
       <c r="L30" s="74"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="74" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C31" s="74"/>
       <c r="D31" s="74"/>
@@ -2914,9 +2991,9 @@
       <c r="K31" s="74"/>
       <c r="L31" s="74"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="74" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C32" s="74"/>
       <c r="D32" s="74"/>
@@ -2929,9 +3006,9 @@
       <c r="K32" s="74"/>
       <c r="L32" s="74"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="74" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C33" s="74"/>
       <c r="D33" s="74"/>
@@ -2944,9 +3021,9 @@
       <c r="K33" s="74"/>
       <c r="L33" s="74"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="74" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C34" s="74"/>
       <c r="D34" s="74"/>
@@ -2959,9 +3036,9 @@
       <c r="K34" s="74"/>
       <c r="L34" s="74"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="74" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C35" s="74"/>
       <c r="D35" s="74"/>
@@ -2974,9 +3051,9 @@
       <c r="K35" s="74"/>
       <c r="L35" s="74"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="74" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C36" s="74"/>
       <c r="D36" s="74"/>
@@ -2989,9 +3066,9 @@
       <c r="K36" s="74"/>
       <c r="L36" s="74"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="74" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C37" s="74"/>
       <c r="D37" s="74"/>
@@ -3004,9 +3081,9 @@
       <c r="K37" s="74"/>
       <c r="L37" s="74"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="74" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C38" s="74"/>
       <c r="D38" s="74"/>
@@ -3019,9 +3096,9 @@
       <c r="K38" s="74"/>
       <c r="L38" s="74"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="74" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C39" s="74"/>
       <c r="D39" s="74"/>
@@ -3034,9 +3111,9 @@
       <c r="K39" s="74"/>
       <c r="L39" s="74"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="82" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C40" s="82"/>
       <c r="D40" s="82"/>
@@ -3049,9 +3126,9 @@
       <c r="K40" s="82"/>
       <c r="L40" s="82"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="74" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C41" s="74"/>
       <c r="D41" s="74"/>
@@ -3064,7 +3141,7 @@
       <c r="K41" s="74"/>
       <c r="L41" s="74"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="74"/>
       <c r="C42" s="74"/>
       <c r="D42" s="74"/>
@@ -3077,9 +3154,9 @@
       <c r="K42" s="74"/>
       <c r="L42" s="74"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="74" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C43" s="74"/>
       <c r="D43" s="74"/>
@@ -3092,9 +3169,9 @@
       <c r="K43" s="74"/>
       <c r="L43" s="74"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="74" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C44" s="74"/>
       <c r="D44" s="74"/>
@@ -3107,9 +3184,9 @@
       <c r="K44" s="74"/>
       <c r="L44" s="74"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="74" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C45" s="74"/>
       <c r="D45" s="74"/>
@@ -3122,7 +3199,7 @@
       <c r="K45" s="74"/>
       <c r="L45" s="74"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="74"/>
       <c r="C46" s="74"/>
       <c r="D46" s="74"/>
@@ -3135,9 +3212,9 @@
       <c r="K46" s="74"/>
       <c r="L46" s="74"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="80" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C47" s="80"/>
       <c r="D47" s="80"/>
@@ -3150,9 +3227,9 @@
       <c r="K47" s="80"/>
       <c r="L47" s="80"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="74" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C48" s="74"/>
       <c r="D48" s="74"/>
@@ -3165,7 +3242,7 @@
       <c r="K48" s="74"/>
       <c r="L48" s="74"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="74"/>
       <c r="C49" s="74"/>
       <c r="D49" s="74"/>
@@ -3178,9 +3255,9 @@
       <c r="K49" s="74"/>
       <c r="L49" s="74"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="80" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C50" s="80"/>
       <c r="D50" s="80"/>
@@ -3193,9 +3270,9 @@
       <c r="K50" s="80"/>
       <c r="L50" s="80"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="74" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C51" s="74"/>
       <c r="D51" s="74"/>
@@ -3208,9 +3285,9 @@
       <c r="K51" s="74"/>
       <c r="L51" s="74"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="74" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C52" s="74"/>
       <c r="D52" s="74"/>
@@ -3223,7 +3300,7 @@
       <c r="K52" s="74"/>
       <c r="L52" s="74"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="74"/>
       <c r="C53" s="74"/>
       <c r="D53" s="74"/>
@@ -3236,9 +3313,9 @@
       <c r="K53" s="74"/>
       <c r="L53" s="74"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="80" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C54" s="80"/>
       <c r="D54" s="80"/>
@@ -3251,9 +3328,9 @@
       <c r="K54" s="80"/>
       <c r="L54" s="80"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="74" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C55" s="74"/>
       <c r="D55" s="74"/>
@@ -3266,9 +3343,9 @@
       <c r="K55" s="74"/>
       <c r="L55" s="74"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="74" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C56" s="74"/>
       <c r="D56" s="74"/>
@@ -3281,7 +3358,7 @@
       <c r="K56" s="74"/>
       <c r="L56" s="74"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="74"/>
       <c r="C57" s="74"/>
       <c r="D57" s="74"/>
@@ -3294,9 +3371,9 @@
       <c r="K57" s="74"/>
       <c r="L57" s="74"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="80" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C58" s="80"/>
       <c r="D58" s="80"/>
@@ -3309,9 +3386,9 @@
       <c r="K58" s="80"/>
       <c r="L58" s="80"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="74" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C59" s="74"/>
       <c r="D59" s="74"/>
@@ -3324,7 +3401,7 @@
       <c r="K59" s="74"/>
       <c r="L59" s="74"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="83"/>
       <c r="C60" s="83"/>
       <c r="D60" s="83"/>
@@ -3337,7 +3414,7 @@
       <c r="K60" s="83"/>
       <c r="L60" s="83"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="84"/>
       <c r="C61" s="84"/>
       <c r="D61" s="84"/>

</xml_diff>